<commit_message>
-Color Data set delete -function for winner declaration created
</commit_message>
<xml_diff>
--- a/NumberRule.xlsx
+++ b/NumberRule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Faras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220273B-FCE5-4E2B-809F-AB4B5AB7B857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904D3FA2-CC7E-4F2A-A32E-C54E5C11BB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="L451" sqref="L451"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,13 +402,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -416,16 +416,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>A3+1</f>
-        <v>3</v>
+        <f>A3-1</f>
+        <v>12</v>
       </c>
       <c r="B4">
-        <f>B3+1</f>
-        <v>3</v>
+        <f>B3-1</f>
+        <v>12</v>
       </c>
       <c r="C4">
-        <f>C3+1</f>
-        <v>3</v>
+        <f>C3-1</f>
+        <v>12</v>
       </c>
       <c r="D4">
         <f>D3+1</f>
@@ -434,16 +434,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A13" si="0">A4+1</f>
-        <v>4</v>
+        <f t="shared" ref="A5:A14" si="0">A4-1</f>
+        <v>11</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B14" si="1">B4+1</f>
-        <v>4</v>
+        <f t="shared" ref="B5:B14" si="1">B4-1</f>
+        <v>11</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C14" si="2">C4+1</f>
-        <v>4</v>
+        <f t="shared" ref="C5:C14" si="2">C4-1</f>
+        <v>11</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D68" si="3">D4+1</f>
@@ -453,15 +453,15 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <f t="shared" si="3"/>
@@ -471,15 +471,15 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
@@ -489,15 +489,15 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
@@ -507,15 +507,15 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <f t="shared" si="3"/>
@@ -525,15 +525,15 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
@@ -543,15 +543,15 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
@@ -561,15 +561,15 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
@@ -579,15 +579,15 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
@@ -596,16 +596,16 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>A13+1</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
@@ -665,7 +665,7 @@
         <v>11</v>
       </c>
       <c r="C18">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="C19">
         <f>C18-1</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="C20">
         <f t="shared" ref="C20:C26" si="6">C19-1</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
@@ -719,7 +719,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
@@ -737,7 +737,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <f t="shared" si="3"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <f t="shared" si="3"/>
@@ -773,7 +773,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24">
         <f t="shared" si="3"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <f t="shared" si="3"/>
@@ -809,7 +809,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <f t="shared" si="3"/>

</xml_diff>